<commit_message>
Fix issue #51 move keep variables after meta variables.
</commit_message>
<xml_diff>
--- a/test/master/hfc test01 enum.xlsx
+++ b/test/master/hfc test01 enum.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="24">
   <si>
     <t>Enumerator</t>
   </si>
@@ -955,16 +955,16 @@
         <v>11</v>
       </c>
       <c r="B4" s="0">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="C4" s="0">
-        <v>93</v>
+        <v>0</v>
       </c>
       <c r="D4" s="0">
-        <v>0</v>
+        <v>0.14946237206459045</v>
       </c>
       <c r="E4" s="0">
-        <v>0.14946237206459045</v>
+        <v>0</v>
       </c>
       <c r="F4" s="0">
         <v>0</v>
@@ -979,10 +979,10 @@
         <v>0</v>
       </c>
       <c r="J4" s="0">
-        <v>0</v>
+        <v>100.30931854248047</v>
       </c>
       <c r="K4" s="0">
-        <v>100.30931854248047</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -990,16 +990,16 @@
         <v>12</v>
       </c>
       <c r="B5" s="0">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="C5" s="0">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="D5" s="0">
-        <v>0</v>
+        <v>0.13970588147640228</v>
       </c>
       <c r="E5" s="0">
-        <v>0.13970588147640228</v>
+        <v>0</v>
       </c>
       <c r="F5" s="0">
         <v>0</v>
@@ -1014,10 +1014,10 @@
         <v>0</v>
       </c>
       <c r="J5" s="0">
-        <v>0</v>
+        <v>251.95613098144531</v>
       </c>
       <c r="K5" s="0">
-        <v>251.95613098144531</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -1025,22 +1025,22 @@
         <v>13</v>
       </c>
       <c r="B6" s="0">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="C6" s="0">
-        <v>83</v>
+        <v>0</v>
       </c>
       <c r="D6" s="0">
-        <v>0</v>
+        <v>0.12008032202720642</v>
       </c>
       <c r="E6" s="0">
-        <v>0.12008032202720642</v>
+        <v>0</v>
       </c>
       <c r="F6" s="0">
-        <v>0</v>
+        <v>0.00045641258475370705</v>
       </c>
       <c r="G6" s="0">
-        <v>0.00045641258475370705</v>
+        <v>0</v>
       </c>
       <c r="H6" s="0">
         <v>0</v>
@@ -1049,10 +1049,10 @@
         <v>0</v>
       </c>
       <c r="J6" s="0">
-        <v>0</v>
+        <v>93.167068481445313</v>
       </c>
       <c r="K6" s="0">
-        <v>93.167068481445313</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -1060,16 +1060,16 @@
         <v>14</v>
       </c>
       <c r="B7" s="0">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="C7" s="0">
-        <v>83</v>
+        <v>0</v>
       </c>
       <c r="D7" s="0">
-        <v>0</v>
+        <v>0.14417670667171478</v>
       </c>
       <c r="E7" s="0">
-        <v>0.14417670667171478</v>
+        <v>0</v>
       </c>
       <c r="F7" s="0">
         <v>0</v>
@@ -1084,10 +1084,10 @@
         <v>0</v>
       </c>
       <c r="J7" s="0">
-        <v>0</v>
+        <v>1185.982666015625</v>
       </c>
       <c r="K7" s="0">
-        <v>1185.982666015625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -1095,16 +1095,16 @@
         <v>15</v>
       </c>
       <c r="B8" s="0">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="C8" s="0">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="D8" s="0">
-        <v>0</v>
+        <v>0.14303797483444214</v>
       </c>
       <c r="E8" s="0">
-        <v>0.14303797483444214</v>
+        <v>0</v>
       </c>
       <c r="F8" s="0">
         <v>0</v>
@@ -1113,16 +1113,16 @@
         <v>0</v>
       </c>
       <c r="H8" s="0">
-        <v>0</v>
+        <v>0.00049236830091103911</v>
       </c>
       <c r="I8" s="0">
-        <v>0.00049236830091103911</v>
+        <v>0</v>
       </c>
       <c r="J8" s="0">
-        <v>0</v>
+        <v>431.74197387695312</v>
       </c>
       <c r="K8" s="0">
-        <v>431.74197387695312</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -1130,16 +1130,16 @@
         <v>17</v>
       </c>
       <c r="B9" s="0">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="C9" s="0">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="D9" s="0">
-        <v>0</v>
+        <v>0.15555556118488312</v>
       </c>
       <c r="E9" s="0">
-        <v>0.15555556118488312</v>
+        <v>0</v>
       </c>
       <c r="F9" s="0">
         <v>0</v>
@@ -1154,10 +1154,10 @@
         <v>0</v>
       </c>
       <c r="J9" s="0">
-        <v>0</v>
+        <v>387.17153930664062</v>
       </c>
       <c r="K9" s="0">
-        <v>387.17153930664062</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -1165,16 +1165,16 @@
         <v>18</v>
       </c>
       <c r="B10" s="0">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C10" s="0">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="D10" s="0">
-        <v>0</v>
+        <v>0.15000000596046448</v>
       </c>
       <c r="E10" s="0">
-        <v>0.15000000596046448</v>
+        <v>0</v>
       </c>
       <c r="F10" s="0">
         <v>0</v>
@@ -1189,10 +1189,10 @@
         <v>0</v>
       </c>
       <c r="J10" s="0">
-        <v>0</v>
+        <v>943.264404296875</v>
       </c>
       <c r="K10" s="0">
-        <v>943.264404296875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -1200,16 +1200,16 @@
         <v>19</v>
       </c>
       <c r="B11" s="0">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="C11" s="0">
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="D11" s="0">
-        <v>0</v>
+        <v>0.15740740299224854</v>
       </c>
       <c r="E11" s="0">
-        <v>0.15740740299224854</v>
+        <v>0</v>
       </c>
       <c r="F11" s="0">
         <v>0</v>
@@ -1218,16 +1218,16 @@
         <v>0</v>
       </c>
       <c r="H11" s="0">
-        <v>0</v>
+        <v>0.0058608059771358967</v>
       </c>
       <c r="I11" s="0">
-        <v>0.0058608059771358967</v>
+        <v>0</v>
       </c>
       <c r="J11" s="0">
-        <v>0</v>
+        <v>64.165122985839844</v>
       </c>
       <c r="K11" s="0">
-        <v>64.165122985839844</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -1235,16 +1235,16 @@
         <v>21</v>
       </c>
       <c r="B12" s="0">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="C12" s="0">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="D12" s="0">
-        <v>0</v>
+        <v>0.15256410837173462</v>
       </c>
       <c r="E12" s="0">
-        <v>0.15256410837173462</v>
+        <v>0</v>
       </c>
       <c r="F12" s="0">
         <v>0</v>
@@ -1253,16 +1253,16 @@
         <v>0</v>
       </c>
       <c r="H12" s="0">
-        <v>0</v>
+        <v>0.0020171457435935736</v>
       </c>
       <c r="I12" s="0">
-        <v>0.0020171457435935736</v>
+        <v>0</v>
       </c>
       <c r="J12" s="0">
-        <v>0</v>
+        <v>1723.4061279296875</v>
       </c>
       <c r="K12" s="0">
-        <v>1723.4061279296875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -1270,16 +1270,16 @@
         <v>22</v>
       </c>
       <c r="B13" s="0">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="C13" s="0">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="D13" s="0">
-        <v>0</v>
+        <v>0.13375000655651093</v>
       </c>
       <c r="E13" s="0">
-        <v>0.13375000655651093</v>
+        <v>0</v>
       </c>
       <c r="F13" s="0">
         <v>0</v>
@@ -1288,16 +1288,16 @@
         <v>0</v>
       </c>
       <c r="H13" s="0">
-        <v>0</v>
+        <v>0.00048100049025379121</v>
       </c>
       <c r="I13" s="0">
-        <v>0.00048100049025379121</v>
+        <v>0</v>
       </c>
       <c r="J13" s="0">
-        <v>0</v>
+        <v>221.09979248046875</v>
       </c>
       <c r="K13" s="0">
-        <v>221.09979248046875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -1305,22 +1305,22 @@
         <v>23</v>
       </c>
       <c r="B14" s="0">
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="C14" s="0">
-        <v>92</v>
+        <v>0</v>
       </c>
       <c r="D14" s="0">
-        <v>0</v>
+        <v>0.20434781908988953</v>
       </c>
       <c r="E14" s="0">
-        <v>0.20434781908988953</v>
+        <v>0</v>
       </c>
       <c r="F14" s="0">
-        <v>0</v>
+        <v>0.00091074680676683784</v>
       </c>
       <c r="G14" s="0">
-        <v>0.00091074680676683784</v>
+        <v>0</v>
       </c>
       <c r="H14" s="0">
         <v>0</v>
@@ -1329,10 +1329,10 @@
         <v>0</v>
       </c>
       <c r="J14" s="0">
-        <v>0</v>
+        <v>70.543838500976563</v>
       </c>
       <c r="K14" s="0">
-        <v>70.543838500976563</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -1340,34 +1340,34 @@
         <v>24</v>
       </c>
       <c r="B15" s="0">
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="C15" s="0">
-        <v>92</v>
+        <v>0</v>
       </c>
       <c r="D15" s="0">
-        <v>0</v>
+        <v>0.14275361597537994</v>
       </c>
       <c r="E15" s="0">
-        <v>0.14275361597537994</v>
+        <v>0</v>
       </c>
       <c r="F15" s="0">
-        <v>0</v>
+        <v>0.0004226542660035193</v>
       </c>
       <c r="G15" s="0">
+        <v>0</v>
+      </c>
+      <c r="H15" s="0">
         <v>0.0004226542660035193</v>
       </c>
-      <c r="H15" s="0">
-        <v>0</v>
-      </c>
       <c r="I15" s="0">
-        <v>0.0004226542660035193</v>
+        <v>0</v>
       </c>
       <c r="J15" s="0">
-        <v>0</v>
+        <v>817.76324462890625</v>
       </c>
       <c r="K15" s="0">
-        <v>817.76324462890625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -1375,16 +1375,16 @@
         <v>25</v>
       </c>
       <c r="B16" s="0">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="C16" s="0">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="D16" s="0">
-        <v>0</v>
+        <v>0.13452380895614624</v>
       </c>
       <c r="E16" s="0">
-        <v>0.13452380895614624</v>
+        <v>0</v>
       </c>
       <c r="F16" s="0">
         <v>0</v>
@@ -1399,10 +1399,10 @@
         <v>0</v>
       </c>
       <c r="J16" s="0">
-        <v>0</v>
+        <v>596.40057373046875</v>
       </c>
       <c r="K16" s="0">
-        <v>596.40057373046875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -1410,16 +1410,16 @@
         <v>26</v>
       </c>
       <c r="B17" s="0">
-        <v>0</v>
+        <v>58</v>
       </c>
       <c r="C17" s="0">
-        <v>58</v>
+        <v>0</v>
       </c>
       <c r="D17" s="0">
-        <v>0</v>
+        <v>0.15689654648303986</v>
       </c>
       <c r="E17" s="0">
-        <v>0.15689654648303986</v>
+        <v>0</v>
       </c>
       <c r="F17" s="0">
         <v>0</v>
@@ -1434,10 +1434,10 @@
         <v>0</v>
       </c>
       <c r="J17" s="0">
-        <v>0</v>
+        <v>55.970401763916016</v>
       </c>
       <c r="K17" s="0">
-        <v>55.970401763916016</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -1445,34 +1445,34 @@
         <v>28</v>
       </c>
       <c r="B18" s="0">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="C18" s="0">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="D18" s="0">
-        <v>0</v>
+        <v>0.11504065245389938</v>
       </c>
       <c r="E18" s="0">
-        <v>0.11504065245389938</v>
+        <v>0</v>
       </c>
       <c r="F18" s="0">
-        <v>0</v>
+        <v>0.0009186954703181982</v>
       </c>
       <c r="G18" s="0">
-        <v>0.0009186954703181982</v>
+        <v>0</v>
       </c>
       <c r="H18" s="0">
-        <v>0</v>
+        <v>0.0004593477351590991</v>
       </c>
       <c r="I18" s="0">
-        <v>0.0004593477351590991</v>
+        <v>0</v>
       </c>
       <c r="J18" s="0">
-        <v>0</v>
+        <v>903.66015625</v>
       </c>
       <c r="K18" s="0">
-        <v>903.66015625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -1480,16 +1480,16 @@
         <v>29</v>
       </c>
       <c r="B19" s="0">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="C19" s="0">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="D19" s="0">
-        <v>0</v>
+        <v>0.1228855699300766</v>
       </c>
       <c r="E19" s="0">
-        <v>0.1228855699300766</v>
+        <v>0</v>
       </c>
       <c r="F19" s="0">
         <v>0</v>
@@ -1498,16 +1498,16 @@
         <v>0</v>
       </c>
       <c r="H19" s="0">
-        <v>0</v>
+        <v>0.00056721497094258666</v>
       </c>
       <c r="I19" s="0">
-        <v>0.00056721497094258666</v>
+        <v>0</v>
       </c>
       <c r="J19" s="0">
-        <v>0</v>
+        <v>343.7955322265625</v>
       </c>
       <c r="K19" s="0">
-        <v>343.7955322265625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -1515,16 +1515,16 @@
         <v>30</v>
       </c>
       <c r="B20" s="0">
-        <v>0</v>
+        <v>79</v>
       </c>
       <c r="C20" s="0">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="D20" s="0">
-        <v>0</v>
+        <v>0.12151898443698883</v>
       </c>
       <c r="E20" s="0">
-        <v>0.12151898443698883</v>
+        <v>0</v>
       </c>
       <c r="F20" s="0">
         <v>0</v>
@@ -1539,10 +1539,10 @@
         <v>0</v>
       </c>
       <c r="J20" s="0">
-        <v>0</v>
+        <v>1072.21875</v>
       </c>
       <c r="K20" s="0">
-        <v>1072.21875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -1550,16 +1550,16 @@
         <v>31</v>
       </c>
       <c r="B21" s="0">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="C21" s="0">
-        <v>91</v>
+        <v>0</v>
       </c>
       <c r="D21" s="0">
-        <v>0</v>
+        <v>0.12380952388048172</v>
       </c>
       <c r="E21" s="0">
-        <v>0.12380952388048172</v>
+        <v>0</v>
       </c>
       <c r="F21" s="0">
         <v>0</v>
@@ -1574,10 +1574,10 @@
         <v>0</v>
       </c>
       <c r="J21" s="0">
-        <v>0</v>
+        <v>150.76263427734375</v>
       </c>
       <c r="K21" s="0">
-        <v>150.76263427734375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -1585,22 +1585,22 @@
         <v>33</v>
       </c>
       <c r="B22" s="0">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="C22" s="0">
-        <v>55</v>
+        <v>0</v>
       </c>
       <c r="D22" s="0">
-        <v>0</v>
+        <v>0.13575758039951324</v>
       </c>
       <c r="E22" s="0">
-        <v>0.13575758039951324</v>
+        <v>0</v>
       </c>
       <c r="F22" s="0">
-        <v>0</v>
+        <v>0.00070126226637512445</v>
       </c>
       <c r="G22" s="0">
-        <v>0.00070126226637512445</v>
+        <v>0</v>
       </c>
       <c r="H22" s="0">
         <v>0</v>
@@ -1609,10 +1609,10 @@
         <v>0</v>
       </c>
       <c r="J22" s="0">
-        <v>0</v>
+        <v>479.41696166992187</v>
       </c>
       <c r="K22" s="0">
-        <v>479.41696166992187</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -1620,16 +1620,16 @@
         <v>34</v>
       </c>
       <c r="B23" s="0">
-        <v>0</v>
+        <v>87</v>
       </c>
       <c r="C23" s="0">
-        <v>87</v>
+        <v>0</v>
       </c>
       <c r="D23" s="0">
-        <v>0</v>
+        <v>0.14521072804927826</v>
       </c>
       <c r="E23" s="0">
-        <v>0.14521072804927826</v>
+        <v>0</v>
       </c>
       <c r="F23" s="0">
         <v>0</v>
@@ -1644,10 +1644,10 @@
         <v>0</v>
       </c>
       <c r="J23" s="0">
-        <v>0</v>
+        <v>157.00421142578125</v>
       </c>
       <c r="K23" s="0">
-        <v>157.00421142578125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -1655,22 +1655,22 @@
         <v>35</v>
       </c>
       <c r="B24" s="0">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="C24" s="0">
-        <v>68</v>
+        <v>0</v>
       </c>
       <c r="D24" s="0">
-        <v>0</v>
+        <v>0.15392157435417175</v>
       </c>
       <c r="E24" s="0">
-        <v>0.15392157435417175</v>
+        <v>0</v>
       </c>
       <c r="F24" s="0">
-        <v>0</v>
+        <v>0.00057937426026910543</v>
       </c>
       <c r="G24" s="0">
-        <v>0.00057937426026910543</v>
+        <v>0</v>
       </c>
       <c r="H24" s="0">
         <v>0</v>
@@ -1679,10 +1679,10 @@
         <v>0</v>
       </c>
       <c r="J24" s="0">
-        <v>0</v>
+        <v>136.29902648925781</v>
       </c>
       <c r="K24" s="0">
-        <v>136.29902648925781</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -1690,16 +1690,16 @@
         <v>36</v>
       </c>
       <c r="B25" s="0">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="C25" s="0">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="D25" s="0">
-        <v>0</v>
+        <v>0.1227642297744751</v>
       </c>
       <c r="E25" s="0">
-        <v>0.1227642297744751</v>
+        <v>0</v>
       </c>
       <c r="F25" s="0">
         <v>0</v>
@@ -1714,10 +1714,10 @@
         <v>0</v>
       </c>
       <c r="J25" s="0">
-        <v>0</v>
+        <v>292.30914306640625</v>
       </c>
       <c r="K25" s="0">
-        <v>292.30914306640625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -1725,34 +1725,34 @@
         <v>37</v>
       </c>
       <c r="B26" s="0">
-        <v>0</v>
+        <v>76</v>
       </c>
       <c r="C26" s="0">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="D26" s="0">
-        <v>0</v>
+        <v>0.11798245459794998</v>
       </c>
       <c r="E26" s="0">
-        <v>0.11798245459794998</v>
+        <v>0</v>
       </c>
       <c r="F26" s="0">
-        <v>0</v>
+        <v>0.026852311566472054</v>
       </c>
       <c r="G26" s="0">
-        <v>0.026852311566472054</v>
+        <v>0</v>
       </c>
       <c r="H26" s="0">
-        <v>0</v>
+        <v>0.00049726502038538456</v>
       </c>
       <c r="I26" s="0">
-        <v>0.00049726502038538456</v>
+        <v>0</v>
       </c>
       <c r="J26" s="0">
-        <v>0</v>
+        <v>789.1473388671875</v>
       </c>
       <c r="K26" s="0">
-        <v>789.1473388671875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27">
@@ -1760,22 +1760,22 @@
         <v>38</v>
       </c>
       <c r="B27" s="0">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="C27" s="0">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="D27" s="0">
-        <v>0</v>
+        <v>0.13924731314182281</v>
       </c>
       <c r="E27" s="0">
-        <v>0.13924731314182281</v>
+        <v>0</v>
       </c>
       <c r="F27" s="0">
-        <v>0</v>
+        <v>0.006870705634355545</v>
       </c>
       <c r="G27" s="0">
-        <v>0.006870705634355545</v>
+        <v>0</v>
       </c>
       <c r="H27" s="0">
         <v>0</v>
@@ -1784,10 +1784,10 @@
         <v>0</v>
       </c>
       <c r="J27" s="0">
-        <v>0</v>
+        <v>3338.1806640625</v>
       </c>
       <c r="K27" s="0">
-        <v>3338.1806640625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -1795,22 +1795,22 @@
         <v>39</v>
       </c>
       <c r="B28" s="0">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="C28" s="0">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="D28" s="0">
-        <v>0</v>
+        <v>0.16290321946144104</v>
       </c>
       <c r="E28" s="0">
-        <v>0.16290321946144104</v>
+        <v>0</v>
       </c>
       <c r="F28" s="0">
-        <v>0</v>
+        <v>0.0019267823081463575</v>
       </c>
       <c r="G28" s="0">
-        <v>0.0019267823081463575</v>
+        <v>0</v>
       </c>
       <c r="H28" s="0">
         <v>0</v>
@@ -1819,10 +1819,10 @@
         <v>0</v>
       </c>
       <c r="J28" s="0">
-        <v>0</v>
+        <v>2450.714111328125</v>
       </c>
       <c r="K28" s="0">
-        <v>2450.714111328125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -1830,22 +1830,22 @@
         <v>40</v>
       </c>
       <c r="B29" s="0">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="C29" s="0">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="D29" s="0">
-        <v>0</v>
+        <v>0.15156249701976776</v>
       </c>
       <c r="E29" s="0">
-        <v>0.15156249701976776</v>
+        <v>0</v>
       </c>
       <c r="F29" s="0">
-        <v>0</v>
+        <v>0.0018416206585243344</v>
       </c>
       <c r="G29" s="0">
-        <v>0.0018416206585243344</v>
+        <v>0</v>
       </c>
       <c r="H29" s="0">
         <v>0</v>
@@ -1854,10 +1854,10 @@
         <v>0</v>
       </c>
       <c r="J29" s="0">
-        <v>0</v>
+        <v>70.351821899414063</v>
       </c>
       <c r="K29" s="0">
-        <v>70.351821899414063</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30">
@@ -1865,22 +1865,22 @@
         <v>41</v>
       </c>
       <c r="B30" s="0">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="C30" s="0">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="D30" s="0">
-        <v>0</v>
+        <v>0.1428571492433548</v>
       </c>
       <c r="E30" s="0">
-        <v>0.1428571492433548</v>
+        <v>0</v>
       </c>
       <c r="F30" s="0">
-        <v>0</v>
+        <v>0.002222222276031971</v>
       </c>
       <c r="G30" s="0">
-        <v>0.002222222276031971</v>
+        <v>0</v>
       </c>
       <c r="H30" s="0">
         <v>0</v>
@@ -1889,10 +1889,10 @@
         <v>0</v>
       </c>
       <c r="J30" s="0">
-        <v>0</v>
+        <v>151.13191223144531</v>
       </c>
       <c r="K30" s="0">
-        <v>151.13191223144531</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -1900,16 +1900,16 @@
         <v>42</v>
       </c>
       <c r="B31" s="0">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C31" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D31" s="0">
-        <v>0</v>
+        <v>0.1666666716337204</v>
       </c>
       <c r="E31" s="0">
-        <v>0.1666666716337204</v>
+        <v>0</v>
       </c>
       <c r="F31" s="0">
         <v>0</v>
@@ -1924,10 +1924,10 @@
         <v>0</v>
       </c>
       <c r="J31" s="0">
-        <v>0</v>
+        <v>63.083332061767578</v>
       </c>
       <c r="K31" s="0">
-        <v>63.083332061767578</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -1935,34 +1935,34 @@
         <v>43</v>
       </c>
       <c r="B32" s="0">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="C32" s="0">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="D32" s="0">
-        <v>0</v>
+        <v>0.12205128371715546</v>
       </c>
       <c r="E32" s="0">
-        <v>0.12205128371715546</v>
+        <v>0</v>
       </c>
       <c r="F32" s="0">
-        <v>0</v>
+        <v>0.0017523363931104541</v>
       </c>
       <c r="G32" s="0">
-        <v>0.0017523363931104541</v>
+        <v>0</v>
       </c>
       <c r="H32" s="0">
-        <v>0</v>
+        <v>0.00058411213103681803</v>
       </c>
       <c r="I32" s="0">
-        <v>0.00058411213103681803</v>
+        <v>0</v>
       </c>
       <c r="J32" s="0">
-        <v>0</v>
+        <v>3475.75732421875</v>
       </c>
       <c r="K32" s="0">
-        <v>3475.75732421875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -1970,16 +1970,16 @@
         <v>44</v>
       </c>
       <c r="B33" s="0">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="C33" s="0">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="D33" s="0">
-        <v>0</v>
+        <v>0.1428571492433548</v>
       </c>
       <c r="E33" s="0">
-        <v>0.1428571492433548</v>
+        <v>0</v>
       </c>
       <c r="F33" s="0">
         <v>0</v>
@@ -1994,10 +1994,10 @@
         <v>0</v>
       </c>
       <c r="J33" s="0">
-        <v>0</v>
+        <v>83.5047607421875</v>
       </c>
       <c r="K33" s="0">
-        <v>83.5047607421875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -2005,16 +2005,16 @@
         <v>46</v>
       </c>
       <c r="B34" s="0">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="C34" s="0">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="D34" s="0">
-        <v>0</v>
+        <v>0.15686275064945221</v>
       </c>
       <c r="E34" s="0">
-        <v>0.15686275064945221</v>
+        <v>0</v>
       </c>
       <c r="F34" s="0">
         <v>0</v>
@@ -2029,10 +2029,10 @@
         <v>0</v>
       </c>
       <c r="J34" s="0">
-        <v>0</v>
+        <v>82.789215087890625</v>
       </c>
       <c r="K34" s="0">
-        <v>82.789215087890625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -2040,22 +2040,22 @@
         <v>47</v>
       </c>
       <c r="B35" s="0">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="C35" s="0">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="D35" s="0">
-        <v>0</v>
+        <v>0.14901961386203766</v>
       </c>
       <c r="E35" s="0">
-        <v>0.14901961386203766</v>
+        <v>0</v>
       </c>
       <c r="F35" s="0">
-        <v>0</v>
+        <v>0.0011520737316459417</v>
       </c>
       <c r="G35" s="0">
-        <v>0.0011520737316459417</v>
+        <v>0</v>
       </c>
       <c r="H35" s="0">
         <v>0</v>
@@ -2064,10 +2064,10 @@
         <v>0</v>
       </c>
       <c r="J35" s="0">
-        <v>0</v>
+        <v>604.82061767578125</v>
       </c>
       <c r="K35" s="0">
-        <v>604.82061767578125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -2075,22 +2075,22 @@
         <v>48</v>
       </c>
       <c r="B36" s="0">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="C36" s="0">
-        <v>71</v>
+        <v>0</v>
       </c>
       <c r="D36" s="0">
-        <v>0</v>
+        <v>0.12863849103450775</v>
       </c>
       <c r="E36" s="0">
-        <v>0.12863849103450775</v>
+        <v>0</v>
       </c>
       <c r="F36" s="0">
-        <v>0</v>
+        <v>0.0016163793625310063</v>
       </c>
       <c r="G36" s="0">
-        <v>0.0016163793625310063</v>
+        <v>0</v>
       </c>
       <c r="H36" s="0">
         <v>0</v>
@@ -2099,10 +2099,10 @@
         <v>0</v>
       </c>
       <c r="J36" s="0">
-        <v>0</v>
+        <v>3287.52294921875</v>
       </c>
       <c r="K36" s="0">
-        <v>3287.52294921875</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37">
@@ -2110,22 +2110,22 @@
         <v>49</v>
       </c>
       <c r="B37" s="0">
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="C37" s="0">
-        <v>73</v>
+        <v>0</v>
       </c>
       <c r="D37" s="0">
-        <v>0</v>
+        <v>0.11095890402793884</v>
       </c>
       <c r="E37" s="0">
-        <v>0.11095890402793884</v>
+        <v>0</v>
       </c>
       <c r="F37" s="0">
-        <v>0</v>
+        <v>0.0010272213257849216</v>
       </c>
       <c r="G37" s="0">
-        <v>0.0010272213257849216</v>
+        <v>0</v>
       </c>
       <c r="H37" s="0">
         <v>0</v>
@@ -2134,10 +2134,10 @@
         <v>0</v>
       </c>
       <c r="J37" s="0">
-        <v>0</v>
+        <v>115440.1484375</v>
       </c>
       <c r="K37" s="0">
-        <v>115440.1484375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38">
@@ -2145,34 +2145,34 @@
         <v>50</v>
       </c>
       <c r="B38" s="0">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="C38" s="0">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="D38" s="0">
-        <v>0</v>
+        <v>0.15362319350242615</v>
       </c>
       <c r="E38" s="0">
-        <v>0.15362319350242615</v>
+        <v>0</v>
       </c>
       <c r="F38" s="0">
-        <v>0</v>
+        <v>0.00085616437718272209</v>
       </c>
       <c r="G38" s="0">
+        <v>0</v>
+      </c>
+      <c r="H38" s="0">
         <v>0.00085616437718272209</v>
       </c>
-      <c r="H38" s="0">
-        <v>0</v>
-      </c>
       <c r="I38" s="0">
-        <v>0.00085616437718272209</v>
+        <v>0</v>
       </c>
       <c r="J38" s="0">
-        <v>0</v>
+        <v>259.24566650390625</v>
       </c>
       <c r="K38" s="0">
-        <v>259.24566650390625</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -2180,16 +2180,16 @@
         <v>51</v>
       </c>
       <c r="B39" s="0">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="C39" s="0">
-        <v>42</v>
+        <v>0</v>
       </c>
       <c r="D39" s="0">
-        <v>0</v>
+        <v>0.16984127461910248</v>
       </c>
       <c r="E39" s="0">
-        <v>0.16984127461910248</v>
+        <v>0</v>
       </c>
       <c r="F39" s="0">
         <v>0</v>
@@ -2204,10 +2204,10 @@
         <v>0</v>
       </c>
       <c r="J39" s="0">
-        <v>0</v>
+        <v>620.60870361328125</v>
       </c>
       <c r="K39" s="0">
-        <v>620.60870361328125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
@@ -2215,16 +2215,16 @@
         <v>52</v>
       </c>
       <c r="B40" s="0">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="C40" s="0">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="D40" s="0">
-        <v>0</v>
+        <v>0.14166666567325592</v>
       </c>
       <c r="E40" s="0">
-        <v>0.14166666567325592</v>
+        <v>0</v>
       </c>
       <c r="F40" s="0">
         <v>0</v>
@@ -2239,10 +2239,10 @@
         <v>0</v>
       </c>
       <c r="J40" s="0">
-        <v>0</v>
+        <v>946.7296142578125</v>
       </c>
       <c r="K40" s="0">
-        <v>946.7296142578125</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>